<commit_message>
add user & mapping user to asset
</commit_message>
<xml_diff>
--- a/InvSystem/obj/Release/Package/PackageTmp/template/TemplateUploadOri.xlsx
+++ b/InvSystem/obj/Release/Package/PackageTmp/template/TemplateUploadOri.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dede\WORK\Case\Inventory IT\Sample\Others\Sample\Empty\Final\InventorySystem\InvSystem\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89812A84-EB5F-42DF-A0CF-6967A73B2956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2626A0E7-5A51-47DD-910B-DB1027BCA5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1190" yWindow="350" windowWidth="16330" windowHeight="4920" xr2:uid="{1D99F045-E079-4AC9-AE53-31F786CA0A7E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1D99F045-E079-4AC9-AE53-31F786CA0A7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -555,7 +556,7 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Value: Code Reference dengan reference type = Chasing Type
+    Value: Code Reference dengan reference type = Chasing Size
 N001=NA
 N002=Micro
 N003=Mini
@@ -610,7 +611,7 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Value: Code Reference dengan reference type = Unit Watt
+    Value: Code Reference dengan reference type = Camera Resolution
 6001=NA
 6002=1 MP</t>
       </text>
@@ -620,7 +621,7 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Value: Code Reference dengan reference type = Unit Watt
+    Value: Code Reference dengan reference type = Camera Type
 5001=NA
 5002=Outdoor</t>
       </text>
@@ -730,7 +731,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="512">
   <si>
     <t>AssetDesc</t>
   </si>
@@ -895,6 +896,1377 @@
   </si>
   <si>
     <t>FrequencyBand</t>
+  </si>
+  <si>
+    <t>Reference Type</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Type Fungsi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NA </t>
+  </si>
+  <si>
+    <t>Print</t>
+  </si>
+  <si>
+    <t>Print Scan</t>
+  </si>
+  <si>
+    <t>Print Scan Copy</t>
+  </si>
+  <si>
+    <t>Unit Voltage</t>
+  </si>
+  <si>
+    <t>12V</t>
+  </si>
+  <si>
+    <t>24V</t>
+  </si>
+  <si>
+    <t>48V</t>
+  </si>
+  <si>
+    <t>Unit Amps</t>
+  </si>
+  <si>
+    <t>600VA</t>
+  </si>
+  <si>
+    <t>1200VA</t>
+  </si>
+  <si>
+    <t>1400VA</t>
+  </si>
+  <si>
+    <t>2000VA</t>
+  </si>
+  <si>
+    <t>2200VA</t>
+  </si>
+  <si>
+    <t>Unit Watt</t>
+  </si>
+  <si>
+    <t>Camera Type</t>
+  </si>
+  <si>
+    <t>Outdoor (Static)</t>
+  </si>
+  <si>
+    <t>Indoor (Static)</t>
+  </si>
+  <si>
+    <t>Indoor (PTZ)</t>
+  </si>
+  <si>
+    <t>Outdoor (PTZ)</t>
+  </si>
+  <si>
+    <t>Camera Resolution</t>
+  </si>
+  <si>
+    <t>1 MP</t>
+  </si>
+  <si>
+    <t>2 MP</t>
+  </si>
+  <si>
+    <t>3 MP</t>
+  </si>
+  <si>
+    <t>4 MP</t>
+  </si>
+  <si>
+    <t>5 MP</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>A001</t>
+  </si>
+  <si>
+    <t>A002</t>
+  </si>
+  <si>
+    <t>Processing Plant</t>
+  </si>
+  <si>
+    <t>A003</t>
+  </si>
+  <si>
+    <t>Office</t>
+  </si>
+  <si>
+    <t>A004</t>
+  </si>
+  <si>
+    <t>Guest House</t>
+  </si>
+  <si>
+    <t>A005</t>
+  </si>
+  <si>
+    <t>Feedmill</t>
+  </si>
+  <si>
+    <t>A006</t>
+  </si>
+  <si>
+    <t>Hatchery</t>
+  </si>
+  <si>
+    <t>A007</t>
+  </si>
+  <si>
+    <t>Landing Site 1</t>
+  </si>
+  <si>
+    <t>A008</t>
+  </si>
+  <si>
+    <t>Landing Site 2</t>
+  </si>
+  <si>
+    <t>Asset Brand</t>
+  </si>
+  <si>
+    <t>B001</t>
+  </si>
+  <si>
+    <t>B002</t>
+  </si>
+  <si>
+    <t>Lenovo</t>
+  </si>
+  <si>
+    <t>B003</t>
+  </si>
+  <si>
+    <t>Asus</t>
+  </si>
+  <si>
+    <t>B004</t>
+  </si>
+  <si>
+    <t>Acer</t>
+  </si>
+  <si>
+    <t>B005</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>B006</t>
+  </si>
+  <si>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>B007</t>
+  </si>
+  <si>
+    <t>Orico</t>
+  </si>
+  <si>
+    <t>B008</t>
+  </si>
+  <si>
+    <t>Bardi</t>
+  </si>
+  <si>
+    <t>B009</t>
+  </si>
+  <si>
+    <t>IBM</t>
+  </si>
+  <si>
+    <t>B010</t>
+  </si>
+  <si>
+    <t>Fortinet</t>
+  </si>
+  <si>
+    <t>B011</t>
+  </si>
+  <si>
+    <t>Mikrotik</t>
+  </si>
+  <si>
+    <t>B012</t>
+  </si>
+  <si>
+    <t>Unifi</t>
+  </si>
+  <si>
+    <t>B013</t>
+  </si>
+  <si>
+    <t>TP-Link</t>
+  </si>
+  <si>
+    <t>B014</t>
+  </si>
+  <si>
+    <t>D-Link</t>
+  </si>
+  <si>
+    <t>B015</t>
+  </si>
+  <si>
+    <t>Ruijie</t>
+  </si>
+  <si>
+    <t>B016</t>
+  </si>
+  <si>
+    <t>Huawei</t>
+  </si>
+  <si>
+    <t>B017</t>
+  </si>
+  <si>
+    <t>Epson</t>
+  </si>
+  <si>
+    <t>B018</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>B019</t>
+  </si>
+  <si>
+    <t>BenQ</t>
+  </si>
+  <si>
+    <t>B020</t>
+  </si>
+  <si>
+    <t>Hikvision</t>
+  </si>
+  <si>
+    <t>B021</t>
+  </si>
+  <si>
+    <t>Mikrobits</t>
+  </si>
+  <si>
+    <t>B022</t>
+  </si>
+  <si>
+    <t>Cambium</t>
+  </si>
+  <si>
+    <t>B023</t>
+  </si>
+  <si>
+    <t>ICA</t>
+  </si>
+  <si>
+    <t>B024</t>
+  </si>
+  <si>
+    <t>Prolink</t>
+  </si>
+  <si>
+    <t>C001</t>
+  </si>
+  <si>
+    <t>C002</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>C003</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>C004</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>C005</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>C006</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>C007</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>C008</t>
+  </si>
+  <si>
+    <t>Transparant</t>
+  </si>
+  <si>
+    <t>C009</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>C010</t>
+  </si>
+  <si>
+    <t>Grey</t>
+  </si>
+  <si>
+    <t>C011</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>D001</t>
+  </si>
+  <si>
+    <t>D002</t>
+  </si>
+  <si>
+    <t>Intel® Core™ i3</t>
+  </si>
+  <si>
+    <t>D003</t>
+  </si>
+  <si>
+    <t>Intel® Core™ i5</t>
+  </si>
+  <si>
+    <t>D004</t>
+  </si>
+  <si>
+    <t>Intel® Core™ i7</t>
+  </si>
+  <si>
+    <t>D005</t>
+  </si>
+  <si>
+    <t>Intel® Core™ i9</t>
+  </si>
+  <si>
+    <t>D006</t>
+  </si>
+  <si>
+    <t>Intel® Pentium® Silver</t>
+  </si>
+  <si>
+    <t>D007</t>
+  </si>
+  <si>
+    <t>Intel® Pentium® Gold</t>
+  </si>
+  <si>
+    <t>D008</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Intel® Celeron®</t>
+  </si>
+  <si>
+    <t>D009</t>
+  </si>
+  <si>
+    <t>Intel Atom® Seri P</t>
+  </si>
+  <si>
+    <t>D010</t>
+  </si>
+  <si>
+    <t>Intel Atom® Seri C</t>
+  </si>
+  <si>
+    <t>D011</t>
+  </si>
+  <si>
+    <t>Intel® Xeon® D</t>
+  </si>
+  <si>
+    <t>D012</t>
+  </si>
+  <si>
+    <t>Intel® Xeon® W</t>
+  </si>
+  <si>
+    <t>D013</t>
+  </si>
+  <si>
+    <t>Intel® Xeon® E</t>
+  </si>
+  <si>
+    <t>D014</t>
+  </si>
+  <si>
+    <t>AMD Athlon™</t>
+  </si>
+  <si>
+    <t>D015</t>
+  </si>
+  <si>
+    <t>AMD Ryzen™</t>
+  </si>
+  <si>
+    <t>E001</t>
+  </si>
+  <si>
+    <t>E002</t>
+  </si>
+  <si>
+    <t>E003</t>
+  </si>
+  <si>
+    <t>Purple</t>
+  </si>
+  <si>
+    <t>E004</t>
+  </si>
+  <si>
+    <t>E005</t>
+  </si>
+  <si>
+    <t>Type Port</t>
+  </si>
+  <si>
+    <t>F001</t>
+  </si>
+  <si>
+    <t>F002</t>
+  </si>
+  <si>
+    <t>Poe-link</t>
+  </si>
+  <si>
+    <t>F003</t>
+  </si>
+  <si>
+    <t>SC/1 Port</t>
+  </si>
+  <si>
+    <t>F004</t>
+  </si>
+  <si>
+    <t>SC/2 Port</t>
+  </si>
+  <si>
+    <t>F005</t>
+  </si>
+  <si>
+    <t>LC/1 Port</t>
+  </si>
+  <si>
+    <t>F006</t>
+  </si>
+  <si>
+    <t>LC/2 Port</t>
+  </si>
+  <si>
+    <t>F007</t>
+  </si>
+  <si>
+    <t>Analog (Coaxial)</t>
+  </si>
+  <si>
+    <t>F008</t>
+  </si>
+  <si>
+    <t>Hybrid (Analog/Network)</t>
+  </si>
+  <si>
+    <t>F009</t>
+  </si>
+  <si>
+    <t>Network (IP)</t>
+  </si>
+  <si>
+    <t>F010</t>
+  </si>
+  <si>
+    <t>Up-link</t>
+  </si>
+  <si>
+    <t>VGA Type</t>
+  </si>
+  <si>
+    <t>G001</t>
+  </si>
+  <si>
+    <t>G002</t>
+  </si>
+  <si>
+    <t>DDR4</t>
+  </si>
+  <si>
+    <t>G003</t>
+  </si>
+  <si>
+    <t>DDR5</t>
+  </si>
+  <si>
+    <t>Charger Type</t>
+  </si>
+  <si>
+    <t>H001</t>
+  </si>
+  <si>
+    <t>H002</t>
+  </si>
+  <si>
+    <t>KW</t>
+  </si>
+  <si>
+    <t>H003</t>
+  </si>
+  <si>
+    <t>ORIGINAL</t>
+  </si>
+  <si>
+    <t>Screen Size</t>
+  </si>
+  <si>
+    <t>I001</t>
+  </si>
+  <si>
+    <t>I002</t>
+  </si>
+  <si>
+    <t>11 Inchi</t>
+  </si>
+  <si>
+    <t>I003</t>
+  </si>
+  <si>
+    <t>12 Inchi</t>
+  </si>
+  <si>
+    <t>I004</t>
+  </si>
+  <si>
+    <t>13 Inchi</t>
+  </si>
+  <si>
+    <t>I005</t>
+  </si>
+  <si>
+    <t>14 Inchi</t>
+  </si>
+  <si>
+    <t>I006</t>
+  </si>
+  <si>
+    <t>15 Inchi</t>
+  </si>
+  <si>
+    <t>I007</t>
+  </si>
+  <si>
+    <t>16 Inchi</t>
+  </si>
+  <si>
+    <t>I008</t>
+  </si>
+  <si>
+    <t>17 Inchi</t>
+  </si>
+  <si>
+    <t>I009</t>
+  </si>
+  <si>
+    <t>18 Inchi</t>
+  </si>
+  <si>
+    <t>I010</t>
+  </si>
+  <si>
+    <t>19 Inchi</t>
+  </si>
+  <si>
+    <t>I011</t>
+  </si>
+  <si>
+    <t>20 Inchi</t>
+  </si>
+  <si>
+    <t>I012</t>
+  </si>
+  <si>
+    <t>21 Inchi</t>
+  </si>
+  <si>
+    <t>I013</t>
+  </si>
+  <si>
+    <t>22 Inchi</t>
+  </si>
+  <si>
+    <t>I014</t>
+  </si>
+  <si>
+    <t>23 Inchi</t>
+  </si>
+  <si>
+    <t>I015</t>
+  </si>
+  <si>
+    <t>24 Inchi</t>
+  </si>
+  <si>
+    <t>Type System</t>
+  </si>
+  <si>
+    <t>J001</t>
+  </si>
+  <si>
+    <t>J002</t>
+  </si>
+  <si>
+    <t>Managenable</t>
+  </si>
+  <si>
+    <t>J003</t>
+  </si>
+  <si>
+    <t>Unmanagenable</t>
+  </si>
+  <si>
+    <t>Port Quantity</t>
+  </si>
+  <si>
+    <t>K001</t>
+  </si>
+  <si>
+    <t>K002</t>
+  </si>
+  <si>
+    <t>5 Port</t>
+  </si>
+  <si>
+    <t>K003</t>
+  </si>
+  <si>
+    <t>8 Port</t>
+  </si>
+  <si>
+    <t>K004</t>
+  </si>
+  <si>
+    <t>16 Port</t>
+  </si>
+  <si>
+    <t>K005</t>
+  </si>
+  <si>
+    <t>24 Port</t>
+  </si>
+  <si>
+    <t>K006</t>
+  </si>
+  <si>
+    <t>32 Port</t>
+  </si>
+  <si>
+    <t>K007</t>
+  </si>
+  <si>
+    <t>1 Port</t>
+  </si>
+  <si>
+    <t>K008</t>
+  </si>
+  <si>
+    <t>2 Port</t>
+  </si>
+  <si>
+    <t>K009</t>
+  </si>
+  <si>
+    <t>3 Port</t>
+  </si>
+  <si>
+    <t>K010</t>
+  </si>
+  <si>
+    <t>4 Port</t>
+  </si>
+  <si>
+    <t>K011</t>
+  </si>
+  <si>
+    <t>48 Port</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>L001</t>
+  </si>
+  <si>
+    <t>L002</t>
+  </si>
+  <si>
+    <t>Lubuk Naga</t>
+  </si>
+  <si>
+    <t>L003</t>
+  </si>
+  <si>
+    <t>Jakarta</t>
+  </si>
+  <si>
+    <t>L004</t>
+  </si>
+  <si>
+    <t>Ajibata</t>
+  </si>
+  <si>
+    <t>L005</t>
+  </si>
+  <si>
+    <t>Pangambatan</t>
+  </si>
+  <si>
+    <t>L006</t>
+  </si>
+  <si>
+    <t>Lontung</t>
+  </si>
+  <si>
+    <t>L007</t>
+  </si>
+  <si>
+    <t>Sirungkungon</t>
+  </si>
+  <si>
+    <t>L008</t>
+  </si>
+  <si>
+    <t>Silimalombu</t>
+  </si>
+  <si>
+    <t>L009</t>
+  </si>
+  <si>
+    <t>Toshiba</t>
+  </si>
+  <si>
+    <t>L010</t>
+  </si>
+  <si>
+    <t>SFP Port Quantity</t>
+  </si>
+  <si>
+    <t>M001</t>
+  </si>
+  <si>
+    <t>M002</t>
+  </si>
+  <si>
+    <t>M003</t>
+  </si>
+  <si>
+    <t>M004</t>
+  </si>
+  <si>
+    <t>M005</t>
+  </si>
+  <si>
+    <t>Chasing Size</t>
+  </si>
+  <si>
+    <t>N001</t>
+  </si>
+  <si>
+    <t>N002</t>
+  </si>
+  <si>
+    <t>Micro</t>
+  </si>
+  <si>
+    <t>N003</t>
+  </si>
+  <si>
+    <t>Mini</t>
+  </si>
+  <si>
+    <t>N004</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>N005</t>
+  </si>
+  <si>
+    <t>Full</t>
+  </si>
+  <si>
+    <t>Operating System</t>
+  </si>
+  <si>
+    <t>O001</t>
+  </si>
+  <si>
+    <t>O002</t>
+  </si>
+  <si>
+    <t>Windows 7</t>
+  </si>
+  <si>
+    <t>O003</t>
+  </si>
+  <si>
+    <t>Windows 8</t>
+  </si>
+  <si>
+    <t>O004</t>
+  </si>
+  <si>
+    <t>Windows 8.1</t>
+  </si>
+  <si>
+    <t>O005</t>
+  </si>
+  <si>
+    <t>Windows 10</t>
+  </si>
+  <si>
+    <t>O006</t>
+  </si>
+  <si>
+    <t>Windows 11</t>
+  </si>
+  <si>
+    <t>O007</t>
+  </si>
+  <si>
+    <t>Windows Ce</t>
+  </si>
+  <si>
+    <t>O008</t>
+  </si>
+  <si>
+    <t>Windows Server 2008</t>
+  </si>
+  <si>
+    <t>O009</t>
+  </si>
+  <si>
+    <t>Windows Server 2008 R2</t>
+  </si>
+  <si>
+    <t>O010</t>
+  </si>
+  <si>
+    <t>Windows Server 2012</t>
+  </si>
+  <si>
+    <t>O011</t>
+  </si>
+  <si>
+    <t>Windows Server 2012 R2</t>
+  </si>
+  <si>
+    <t>O012</t>
+  </si>
+  <si>
+    <t>Windows Server 2016</t>
+  </si>
+  <si>
+    <t>O013</t>
+  </si>
+  <si>
+    <t>Windows Server 2016 R2</t>
+  </si>
+  <si>
+    <t>O014</t>
+  </si>
+  <si>
+    <t>Linux Centos</t>
+  </si>
+  <si>
+    <t>O015</t>
+  </si>
+  <si>
+    <t>VMware Esxi 6.7.0</t>
+  </si>
+  <si>
+    <t>O016</t>
+  </si>
+  <si>
+    <t>VMware Esxi 6.5.0</t>
+  </si>
+  <si>
+    <t>Placement Characteristic</t>
+  </si>
+  <si>
+    <t>P001</t>
+  </si>
+  <si>
+    <t>P002</t>
+  </si>
+  <si>
+    <t>Stationary</t>
+  </si>
+  <si>
+    <t>P003</t>
+  </si>
+  <si>
+    <t>Carry By Employee</t>
+  </si>
+  <si>
+    <t>Type Quality</t>
+  </si>
+  <si>
+    <t>Q001</t>
+  </si>
+  <si>
+    <t>Q002</t>
+  </si>
+  <si>
+    <t>10/100</t>
+  </si>
+  <si>
+    <t>Q003</t>
+  </si>
+  <si>
+    <t>10/100/1000</t>
+  </si>
+  <si>
+    <t>Q004</t>
+  </si>
+  <si>
+    <t>10/100/1000/10000</t>
+  </si>
+  <si>
+    <t>RAM Type</t>
+  </si>
+  <si>
+    <t>R001</t>
+  </si>
+  <si>
+    <t>R002</t>
+  </si>
+  <si>
+    <t>DDR</t>
+  </si>
+  <si>
+    <t>R003</t>
+  </si>
+  <si>
+    <t>DDR2</t>
+  </si>
+  <si>
+    <t>R004</t>
+  </si>
+  <si>
+    <t>DDR3</t>
+  </si>
+  <si>
+    <t>R005</t>
+  </si>
+  <si>
+    <t>DDR3L</t>
+  </si>
+  <si>
+    <t>R006</t>
+  </si>
+  <si>
+    <t>R007</t>
+  </si>
+  <si>
+    <t>Storage Type</t>
+  </si>
+  <si>
+    <t>T001</t>
+  </si>
+  <si>
+    <t>T002</t>
+  </si>
+  <si>
+    <t>Harddisk (HDD)</t>
+  </si>
+  <si>
+    <t>T003</t>
+  </si>
+  <si>
+    <t>Solid State Drive (SSD-Nvme)</t>
+  </si>
+  <si>
+    <t>T004</t>
+  </si>
+  <si>
+    <t>Solid State Drive (SSD-Nvme M.2)</t>
+  </si>
+  <si>
+    <t>T005</t>
+  </si>
+  <si>
+    <t>Solid State Drive (Sata 3)</t>
+  </si>
+  <si>
+    <t>Touch Screen</t>
+  </si>
+  <si>
+    <t>U001</t>
+  </si>
+  <si>
+    <t>U002</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>U003</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>VGA Brand</t>
+  </si>
+  <si>
+    <t>V001</t>
+  </si>
+  <si>
+    <t>V002</t>
+  </si>
+  <si>
+    <t>NVidia</t>
+  </si>
+  <si>
+    <t>V003</t>
+  </si>
+  <si>
+    <t>Radeon</t>
+  </si>
+  <si>
+    <t>V004</t>
+  </si>
+  <si>
+    <t>ATI Radeon</t>
+  </si>
+  <si>
+    <t>V005</t>
+  </si>
+  <si>
+    <t>Intel Iris</t>
+  </si>
+  <si>
+    <t>V006</t>
+  </si>
+  <si>
+    <t>Intel</t>
+  </si>
+  <si>
+    <t>Frequency Band</t>
+  </si>
+  <si>
+    <t>W001</t>
+  </si>
+  <si>
+    <t>W002</t>
+  </si>
+  <si>
+    <t>2.4 Ghz</t>
+  </si>
+  <si>
+    <t>W003</t>
+  </si>
+  <si>
+    <t>5 Ghz</t>
+  </si>
+  <si>
+    <t>W004</t>
+  </si>
+  <si>
+    <t>6 Ghz</t>
+  </si>
+  <si>
+    <t>Type Connectivity</t>
+  </si>
+  <si>
+    <t>X001</t>
+  </si>
+  <si>
+    <t>X002</t>
+  </si>
+  <si>
+    <t>Wired</t>
+  </si>
+  <si>
+    <t>X003</t>
+  </si>
+  <si>
+    <t>Wirelless</t>
+  </si>
+  <si>
+    <t>X004</t>
+  </si>
+  <si>
+    <t>Direct</t>
+  </si>
+  <si>
+    <t>X005</t>
+  </si>
+  <si>
+    <t>USB Port</t>
+  </si>
+  <si>
+    <t>Battery Type</t>
+  </si>
+  <si>
+    <t>Y001</t>
+  </si>
+  <si>
+    <t>Y002</t>
+  </si>
+  <si>
+    <t>Internal</t>
+  </si>
+  <si>
+    <t>Y003</t>
+  </si>
+  <si>
+    <t>External</t>
+  </si>
+  <si>
+    <t>Screen Resolution</t>
+  </si>
+  <si>
+    <t>Z001</t>
+  </si>
+  <si>
+    <t>Z002</t>
+  </si>
+  <si>
+    <t>1024 x 768</t>
+  </si>
+  <si>
+    <t>Z003</t>
+  </si>
+  <si>
+    <t>1152 x 864</t>
+  </si>
+  <si>
+    <t>Z004</t>
+  </si>
+  <si>
+    <t>1280 x 600</t>
+  </si>
+  <si>
+    <t>Z005</t>
+  </si>
+  <si>
+    <t>1280 x 720</t>
+  </si>
+  <si>
+    <t>Asset Type</t>
+  </si>
+  <si>
+    <t>S001</t>
+  </si>
+  <si>
+    <t>S002</t>
+  </si>
+  <si>
+    <t>Laptop</t>
+  </si>
+  <si>
+    <t>S003</t>
+  </si>
+  <si>
+    <t>Printer Wirelless</t>
+  </si>
+  <si>
+    <t>S004</t>
+  </si>
+  <si>
+    <t>Projector</t>
+  </si>
+  <si>
+    <t>S005</t>
+  </si>
+  <si>
+    <t>Router</t>
+  </si>
+  <si>
+    <t>S006</t>
+  </si>
+  <si>
+    <t>Access Point</t>
+  </si>
+  <si>
+    <t>S007</t>
+  </si>
+  <si>
+    <t>UPS</t>
+  </si>
+  <si>
+    <t>S008</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>S009</t>
+  </si>
+  <si>
+    <t>Camera Coaxial</t>
+  </si>
+  <si>
+    <t>S010</t>
+  </si>
+  <si>
+    <t>Closed Circuit Television (CCTV)</t>
+  </si>
+  <si>
+    <t>S011</t>
+  </si>
+  <si>
+    <t>Digital Video Recorder (DVR)</t>
+  </si>
+  <si>
+    <t>S012</t>
+  </si>
+  <si>
+    <t>Network Video Recorder (NVR)</t>
+  </si>
+  <si>
+    <t>S013</t>
+  </si>
+  <si>
+    <t>Switch 10/100</t>
+  </si>
+  <si>
+    <t>S014</t>
+  </si>
+  <si>
+    <t>Hybrid Video Recorder (HVR)</t>
+  </si>
+  <si>
+    <t>S015</t>
+  </si>
+  <si>
+    <t>Module Converter (MC)</t>
+  </si>
+  <si>
+    <t>S016</t>
+  </si>
+  <si>
+    <t>Printer</t>
+  </si>
+  <si>
+    <t>S017</t>
+  </si>
+  <si>
+    <t>Printer Lan</t>
+  </si>
+  <si>
+    <t>S018</t>
+  </si>
+  <si>
+    <t>Stabillizer</t>
+  </si>
+  <si>
+    <t>S019</t>
+  </si>
+  <si>
+    <t>HDD Casing 2.4</t>
+  </si>
+  <si>
+    <t>S020</t>
+  </si>
+  <si>
+    <t>HDD Casing 3.5</t>
+  </si>
+  <si>
+    <t>S021</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>S022</t>
+  </si>
+  <si>
+    <t>Battery</t>
+  </si>
+  <si>
+    <t>S023</t>
+  </si>
+  <si>
+    <t>Scanner</t>
+  </si>
+  <si>
+    <t>S024</t>
+  </si>
+  <si>
+    <t>Module SFP</t>
+  </si>
+  <si>
+    <t>S025</t>
+  </si>
+  <si>
+    <t>Module Converter</t>
+  </si>
+  <si>
+    <t>S026</t>
+  </si>
+  <si>
+    <t>Modem</t>
+  </si>
+  <si>
+    <t>S027</t>
+  </si>
+  <si>
+    <t>Storage External</t>
+  </si>
+  <si>
+    <t>S028</t>
+  </si>
+  <si>
+    <t>Computer Dekstop</t>
+  </si>
+  <si>
+    <t>S029</t>
+  </si>
+  <si>
+    <t>Barcode Scanner</t>
+  </si>
+  <si>
+    <t>NIK</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - </t>
+  </si>
+  <si>
+    <t>Dede Wahinime Antini</t>
   </si>
 </sst>
 </file>
@@ -913,21 +2285,35 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor theme="8" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -935,13 +2321,59 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="8" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="8" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="8" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="8" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="8" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="8" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="8" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="8" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -963,6 +2395,39 @@
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <person displayName="Dede W. Antini" id="{B454E715-2E34-4181-B687-C2802F0FA090}" userId="S::dede.antini@regalsprings.com::5d34fccf-4c4c-4076-94fa-6ff9a19c42f1" providerId="AD"/>
 </personList>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6243546D-69D0-4B28-BE7C-3651E1FB8810}" name="Table1" displayName="Table1" ref="A1:C5" totalsRowShown="0">
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{21181D31-5A02-4E87-8CF2-625D2C244263}" name="Reference Type"/>
+    <tableColumn id="2" xr3:uid="{EC271AF4-AAA5-4510-B6A7-5B5D6B3C70FA}" name="Code"/>
+    <tableColumn id="3" xr3:uid="{6173810A-372A-4DD3-A9D4-B6026EA1664B}" name="Name"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E94EA782-40F8-45F9-BB9A-35FAB288F8DA}" name="Table2" displayName="Table2" ref="DU1:DW30" totalsRowShown="0">
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{07FCFFC2-4141-4681-B516-C2F5B440F96F}" name="Reference Type"/>
+    <tableColumn id="2" xr3:uid="{CC5DBBCE-7A83-4AC4-80FF-30878A107716}" name="Code"/>
+    <tableColumn id="3" xr3:uid="{F532FB10-4ED1-448E-876C-15D88E38D319}" name="Name"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{15E4EB1C-D8B0-4EA6-AFA0-9FCB4A23467D}" name="Table3" displayName="Table3" ref="DY1:EA3" totalsRowShown="0">
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{13509954-D920-4B99-AAB1-E3FB72BE0C8C}" name="Reference Type"/>
+    <tableColumn id="2" xr3:uid="{98B4C5FF-CBDE-4B7D-A080-2C39F09A5B1B}" name="NIK"/>
+    <tableColumn id="3" xr3:uid="{51FCDD8A-3040-43B2-A1F6-C4085C090F0E}" name="Name"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1535,7 +3000,7 @@
     <text>Length: 300 character</text>
   </threadedComment>
   <threadedComment ref="AL1" dT="2022-11-25T02:30:10.26" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{A428C808-FB23-4D94-8784-ABA1CEE99BDD}">
-    <text>Value: Code Reference dengan reference type = Chasing Type
+    <text>Value: Code Reference dengan reference type = Chasing Size
 N001=NA
 N002=Micro
 N003=Mini
@@ -1565,12 +3030,12 @@
 4003=600</text>
   </threadedComment>
   <threadedComment ref="AQ1" dT="2022-11-25T02:29:40.41" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{60EF7FD3-3C14-42CD-B72B-D2C5F8E0620D}">
-    <text>Value: Code Reference dengan reference type = Unit Watt
+    <text>Value: Code Reference dengan reference type = Camera Resolution
 6001=NA
 6002=1 MP</text>
   </threadedComment>
   <threadedComment ref="AR1" dT="2022-11-25T02:30:26.68" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{8C293A15-0351-42E6-8CA8-98C96A5A6B59}">
-    <text>Value: Code Reference dengan reference type = Unit Watt
+    <text>Value: Code Reference dengan reference type = Camera Type
 5001=NA
 5002=Outdoor</text>
   </threadedComment>
@@ -1626,8 +3091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD97E317-5A98-407F-9C59-B1011D36E470}">
   <dimension ref="A1:BC1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
-      <selection activeCell="AY1" sqref="AY1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1635,6 +3100,7 @@
     <col min="1" max="1" width="16.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:55" x14ac:dyDescent="0.35">
@@ -1808,5 +3274,2869 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="34">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{521E17A4-9DFB-41CD-9EFC-0542F62610D7}">
+          <x14:formula1>
+            <xm:f>Sheet2!$AP$2:$AP$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CA94F24C-8A71-42A3-B092-8EABCE6388D4}">
+          <x14:formula1>
+            <xm:f>Sheet2!$CH$2:$CH$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8611EC89-E625-43F3-9570-7458A6508249}">
+          <x14:formula1>
+            <xm:f>Sheet2!$BR$2:$BR$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F991CA15-A1AF-4E9D-BB68-B88BB753BCA0}">
+          <x14:formula1>
+            <xm:f>Sheet2!$Z$2:$Z$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{94C39EA4-8058-4A49-997A-F40008F374D7}">
+          <x14:formula1>
+            <xm:f>Sheet2!$DV$2:$DV$30</xm:f>
+          </x14:formula1>
+          <xm:sqref>K2:K1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A9C64B6C-3B55-4374-9CA6-CFDFB6767C90}">
+          <x14:formula1>
+            <xm:f>Sheet2!$AD$2:$AD$25</xm:f>
+          </x14:formula1>
+          <xm:sqref>L2:L1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DAB918C3-32A7-4CB1-B8D6-8945BF94AA54}">
+          <x14:formula1>
+            <xm:f>Sheet2!$AH$2:$AH$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>P2:P1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{55265129-7763-48E8-A2E8-1D2C960259C2}">
+          <x14:formula1>
+            <xm:f>Sheet2!$AL$2:$AL$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>R2:R1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{38665F7C-79C6-4BC0-A492-AA437FA8EF1A}">
+          <x14:formula1>
+            <xm:f>Sheet2!$CD$2:$CD$17</xm:f>
+          </x14:formula1>
+          <xm:sqref>S2:S1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{29827F6A-DF10-441B-9F21-62D8CAB18596}">
+          <x14:formula1>
+            <xm:f>Sheet2!$DJ$2:$DJ$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>T3:T1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{7575A936-EA4C-4507-8F73-8D25B97E2E20}">
+          <x14:formula1>
+            <xm:f>Sheet2!$DJ$2:$DJ$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>T2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0AC98AF1-AAA7-40F8-9036-EE056B1062D8}">
+          <x14:formula1>
+            <xm:f>Sheet2!$B$2:$B$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>U2:U1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{826B1AB0-19EB-44B4-9F43-8CBF5F2B2975}">
+          <x14:formula1>
+            <xm:f>Sheet2!$BF$2:$BF$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>V2:V1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EAE33CFA-E538-4386-80AA-5DDECD52C280}">
+          <x14:formula1>
+            <xm:f>Sheet2!$DR$2:$DR$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>W2:W1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9B13FC53-D235-4C49-9CD3-EDB0D802E050}">
+          <x14:formula1>
+            <xm:f>Sheet2!$CX$2:$CX$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>X2:X1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7700E988-AD28-4AD5-9C64-A428C00E9F6E}">
+          <x14:formula1>
+            <xm:f>Sheet2!$DB$2:$DB$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>Y2:Y1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0E7A52F6-2525-43B4-8E6B-21DA8BE6C30B}">
+          <x14:formula1>
+            <xm:f>Sheet2!$AX$2:$AX$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>Z2:Z1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{05BA50E4-1D99-42C2-BE3A-F7058AED263C}">
+          <x14:formula1>
+            <xm:f>Sheet2!$CP$2:$CP$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>AB2:AB1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3402851A-1298-4E82-BE6D-9DBE3A598215}">
+          <x14:formula1>
+            <xm:f>Sheet2!$CT$2:$CT$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>AE2:AE1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B04777D6-94AE-4035-A443-536C36BC5185}">
+          <x14:formula1>
+            <xm:f>Sheet2!$BB$2:$BB$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>AG2:AG1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ECC9D203-13CE-49DC-AB50-0CDD675D5666}">
+          <x14:formula1>
+            <xm:f>Sheet2!$F$2:$F$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>AH2:AH1048576 AN2:AN1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{509E37FC-20F7-45C2-A4F9-E7D0975531B7}">
+          <x14:formula1>
+            <xm:f>Sheet2!$J$2:$J$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>AI2:AI1048576 AO2:AO1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C0A5E419-86FF-439B-952A-F3DC993CB3A0}">
+          <x14:formula1>
+            <xm:f>Sheet2!$N$2:$N$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>AJ2:AJ1048576 AP2:AP1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BA6A778B-617C-4C99-89AC-BAF506465CED}">
+          <x14:formula1>
+            <xm:f>Sheet2!$BZ$2:$BZ$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>AL2:AL1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3DF47C9C-EA86-4E0F-888F-E75182DA39E2}">
+          <x14:formula1>
+            <xm:f>Sheet2!$DN$2:$DN$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>AM2:AM1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00465D4C-7494-4DC8-8A7B-5DA4A3AC327D}">
+          <x14:formula1>
+            <xm:f>Sheet2!$V$2:$V$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>AQ2:AQ1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9EF843E3-A61B-4A0F-A947-1CB5F3150AC6}">
+          <x14:formula1>
+            <xm:f>Sheet2!$R$2:$R$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>AR2:AR1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FF5C6804-0149-4B4F-9B30-E334FFA61F31}">
+          <x14:formula1>
+            <xm:f>Sheet2!$CL$2:$CL$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>AS2:AS1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FEA19404-387A-496A-B92D-AB0004A37C79}">
+          <x14:formula1>
+            <xm:f>Sheet2!$AT$2:$AT$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>AT2:AT1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{48C62BBA-ECB4-468C-9254-5300B2160B34}">
+          <x14:formula1>
+            <xm:f>Sheet2!$BJ$2:$BJ$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>AU2:AU1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DD0B385C-1FA3-4A21-B7AC-FD6259D74B86}">
+          <x14:formula1>
+            <xm:f>Sheet2!$BN$2:$BN$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>AV2:AV1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B68344A5-62CD-4288-8746-D25BC63C3EF7}">
+          <x14:formula1>
+            <xm:f>Sheet2!$BV$2:$BV$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>AW2:AW1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{58A443D1-EA20-4553-9BD1-2C415C7982FA}">
+          <x14:formula1>
+            <xm:f>Sheet2!$DF$2:$DF$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>AX2:AX1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E2E0CB50-4087-47B7-BF44-BFBD9BCA0117}">
+          <x14:formula1>
+            <xm:f>Sheet2!$DZ$2:$DZ$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>J2:J1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77814C16-67B4-433D-A132-47DC7CB73876}">
+  <dimension ref="A1:EA30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.6328125" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.90625" customWidth="1"/>
+    <col min="9" max="9" width="12.08984375" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="17" max="17" width="11.453125" customWidth="1"/>
+    <col min="21" max="21" width="16.453125" customWidth="1"/>
+    <col min="27" max="27" width="13.6328125" customWidth="1"/>
+    <col min="29" max="29" width="11.7265625" customWidth="1"/>
+    <col min="35" max="35" width="10.7265625" customWidth="1"/>
+    <col min="39" max="39" width="19.36328125" customWidth="1"/>
+    <col min="47" max="47" width="22.7265625" customWidth="1"/>
+    <col min="49" max="49" width="11.36328125" customWidth="1"/>
+    <col min="53" max="53" width="14.36328125" customWidth="1"/>
+    <col min="57" max="57" width="12.36328125" customWidth="1"/>
+    <col min="65" max="65" width="14" customWidth="1"/>
+    <col min="71" max="71" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="20.90625" customWidth="1"/>
+    <col min="87" max="87" width="16.7265625" customWidth="1"/>
+    <col min="89" max="89" width="11.1796875" customWidth="1"/>
+    <col min="91" max="91" width="16.90625" customWidth="1"/>
+    <col min="97" max="97" width="11.6328125" customWidth="1"/>
+    <col min="99" max="99" width="28.6328125" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="15.6328125" customWidth="1"/>
+    <col min="127" max="127" width="27.1796875" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="15.6328125" customWidth="1"/>
+    <col min="130" max="130" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="19.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:131" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AP1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AT1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AX1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AY1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="BA1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="BB1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="BC1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="BE1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="BF1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="BG1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="BI1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="BJ1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="BK1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="BM1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="BN1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="BO1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="BQ1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="BR1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="BS1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="BU1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="BV1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="BW1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="BY1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="BZ1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="CA1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="CC1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="CD1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="CE1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="CG1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="CH1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="CI1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="CK1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="CL1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="CM1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="CO1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="CP1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="CQ1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="CS1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="CT1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="CU1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="CW1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="CX1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="CY1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="DA1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="DB1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="DC1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="DE1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="DF1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="DG1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="DI1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="DJ1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="DK1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="DM1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="DN1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="DO1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="DQ1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="DR1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="DS1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="DU1" t="s">
+        <v>55</v>
+      </c>
+      <c r="DV1" t="s">
+        <v>56</v>
+      </c>
+      <c r="DW1" t="s">
+        <v>57</v>
+      </c>
+      <c r="DY1" t="s">
+        <v>55</v>
+      </c>
+      <c r="DZ1" t="s">
+        <v>508</v>
+      </c>
+      <c r="EA1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:131" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2">
+        <v>1001</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="6">
+        <v>2001</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J2" s="6">
+        <v>3001</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="N2" s="6">
+        <v>4001</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="R2" s="6">
+        <v>5001</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="V2" s="9">
+        <v>6001</v>
+      </c>
+      <c r="W2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y2" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z2" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC2" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD2" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH2" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="AI2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL2" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="AM2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AO2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP2" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="AQ2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS2" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="AT2" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="AU2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AW2" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="AX2" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="AY2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="BA2" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="BB2" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="BC2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="BE2" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="BF2" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="BG2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="BI2" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="BJ2" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="BK2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="BM2" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="BN2" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="BO2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="BQ2" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="BR2" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="BS2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="BU2" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="BV2" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="BW2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="BY2" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="BZ2" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="CA2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="CC2" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="CD2" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="CE2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="CG2" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="CH2" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="CI2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="CK2" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="CL2" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="CM2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="CO2" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="CP2" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="CQ2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="CS2" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="CT2" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="CU2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="CW2" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="CX2" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="CY2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="DA2" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="DB2" s="9" t="s">
+        <v>405</v>
+      </c>
+      <c r="DC2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="DE2" s="8" t="s">
+        <v>416</v>
+      </c>
+      <c r="DF2" s="9" t="s">
+        <v>417</v>
+      </c>
+      <c r="DG2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="DI2" s="8" t="s">
+        <v>424</v>
+      </c>
+      <c r="DJ2" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="DK2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="DM2" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="DN2" s="6" t="s">
+        <v>435</v>
+      </c>
+      <c r="DO2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="DQ2" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="DR2" s="9" t="s">
+        <v>441</v>
+      </c>
+      <c r="DS2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="DU2" t="s">
+        <v>450</v>
+      </c>
+      <c r="DV2" t="s">
+        <v>451</v>
+      </c>
+      <c r="DW2" t="s">
+        <v>59</v>
+      </c>
+      <c r="DY2" t="s">
+        <v>43</v>
+      </c>
+      <c r="DZ2" t="s">
+        <v>509</v>
+      </c>
+      <c r="EA2" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="3" spans="1:131" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3">
+        <v>1002</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="9">
+        <v>2002</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" s="9">
+        <v>3002</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="N3" s="9">
+        <v>4002</v>
+      </c>
+      <c r="O3" s="10">
+        <v>300</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="R3" s="9">
+        <v>5002</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="V3" s="6">
+        <v>6002</v>
+      </c>
+      <c r="W3" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z3" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA3" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="AC3" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD3" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="AE3" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH3" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="AI3" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL3" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="AM3" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="AO3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP3" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="AQ3" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="AS3" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="AT3" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="AU3" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="AW3" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="AX3" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="AY3" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="BA3" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="BB3" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="BC3" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="BE3" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="BF3" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="BG3" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="BI3" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="BJ3" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="BK3" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="BM3" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="BN3" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="BO3" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="BQ3" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="BR3" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="BS3" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="BU3" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="BV3" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="BW3" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="BY3" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="BZ3" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="CA3" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="CC3" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="CD3" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="CE3" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="CG3" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="CH3" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="CI3" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="CK3" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="CL3" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="CM3" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="CO3" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="CP3" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="CQ3" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="CS3" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="CT3" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="CU3" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="CW3" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="CX3" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="CY3" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="DA3" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="DB3" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="DC3" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="DE3" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="DF3" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="DG3" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="DI3" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="DJ3" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="DK3" s="7" t="s">
+        <v>427</v>
+      </c>
+      <c r="DM3" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="DN3" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="DO3" s="10" t="s">
+        <v>437</v>
+      </c>
+      <c r="DQ3" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="DR3" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="DS3" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="DU3" t="s">
+        <v>450</v>
+      </c>
+      <c r="DV3" t="s">
+        <v>452</v>
+      </c>
+      <c r="DW3" t="s">
+        <v>453</v>
+      </c>
+      <c r="DY3" t="s">
+        <v>43</v>
+      </c>
+      <c r="DZ3">
+        <v>2020120170</v>
+      </c>
+      <c r="EA3" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="4" spans="1:131" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4">
+        <v>1003</v>
+      </c>
+      <c r="C4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="6">
+        <v>2003</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J4" s="6">
+        <v>3003</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="N4" s="6">
+        <v>4003</v>
+      </c>
+      <c r="O4" s="7">
+        <v>600</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="R4" s="6">
+        <v>5003</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="U4" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="V4" s="9">
+        <v>6003</v>
+      </c>
+      <c r="W4" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y4" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z4" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA4" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC4" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD4" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="AE4" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="AG4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH4" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="AI4" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="AK4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL4" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="AM4" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="AO4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP4" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="AQ4" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="AS4" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="AT4" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="AU4" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="AW4" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="AX4" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="AY4" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="BA4" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="BB4" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="BC4" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="BE4" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="BF4" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="BG4" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="BI4" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="BJ4" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="BK4" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="BM4" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="BN4" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="BO4" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="BQ4" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="BR4" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="BS4" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="BU4" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="BV4" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="BW4" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="BY4" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="BZ4" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="CA4" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="CC4" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="CD4" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="CE4" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="CG4" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="CH4" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="CI4" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="CK4" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="CL4" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="CM4" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="CO4" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="CP4" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="CQ4" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="CS4" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="CT4" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="CU4" s="10" t="s">
+        <v>393</v>
+      </c>
+      <c r="CW4" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="CX4" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="CY4" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="DA4" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="DB4" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="DC4" s="10" t="s">
+        <v>409</v>
+      </c>
+      <c r="DE4" s="8" t="s">
+        <v>416</v>
+      </c>
+      <c r="DF4" s="9" t="s">
+        <v>420</v>
+      </c>
+      <c r="DG4" s="10" t="s">
+        <v>421</v>
+      </c>
+      <c r="DI4" s="8" t="s">
+        <v>424</v>
+      </c>
+      <c r="DJ4" s="9" t="s">
+        <v>428</v>
+      </c>
+      <c r="DK4" s="10" t="s">
+        <v>429</v>
+      </c>
+      <c r="DM4" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="DN4" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="DO4" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="DQ4" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="DR4" s="9" t="s">
+        <v>444</v>
+      </c>
+      <c r="DS4" s="10" t="s">
+        <v>445</v>
+      </c>
+      <c r="DU4" t="s">
+        <v>450</v>
+      </c>
+      <c r="DV4" t="s">
+        <v>454</v>
+      </c>
+      <c r="DW4" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="5" spans="1:131" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5">
+        <v>1004</v>
+      </c>
+      <c r="C5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="9">
+        <v>2004</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="J5" s="9">
+        <v>3004</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="N5" s="9">
+        <v>4004</v>
+      </c>
+      <c r="O5" s="10">
+        <v>1200</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="R5" s="9">
+        <v>5004</v>
+      </c>
+      <c r="S5" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="V5" s="6">
+        <v>6004</v>
+      </c>
+      <c r="W5" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y5" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z5" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA5" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC5" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD5" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE5" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="AG5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH5" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="AI5" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AK5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL5" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="AM5" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="AO5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP5" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="AQ5" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="AS5" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="AT5" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="AU5" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="BE5" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="BF5" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="BG5" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="BM5" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="BN5" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="BO5" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="BQ5" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="BR5" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="BS5" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="BU5" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="BV5" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="BW5" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="BY5" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="BZ5" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="CA5" s="10" t="s">
+        <v>327</v>
+      </c>
+      <c r="CC5" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="CD5" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="CE5" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="CK5" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="CL5" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="CM5" s="10" t="s">
+        <v>375</v>
+      </c>
+      <c r="CO5" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="CP5" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="CQ5" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="CS5" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="CT5" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="CU5" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="DA5" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="DB5" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="DC5" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="DE5" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="DF5" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="DG5" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="DI5" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="DJ5" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="DK5" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="DQ5" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="DR5" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="DS5" s="7" t="s">
+        <v>447</v>
+      </c>
+      <c r="DU5" t="s">
+        <v>450</v>
+      </c>
+      <c r="DV5" t="s">
+        <v>456</v>
+      </c>
+      <c r="DW5" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="6" spans="1:131" x14ac:dyDescent="0.35">
+      <c r="I6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6" s="6">
+        <v>3005</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="R6" s="6">
+        <v>5005</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="U6" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="V6" s="9">
+        <v>6005</v>
+      </c>
+      <c r="W6" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y6" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z6" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA6" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC6" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD6" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE6" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH6" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="AI6" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="AK6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL6" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="AM6" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="AO6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP6" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="AQ6" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="AS6" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="AT6" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="AU6" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="BE6" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="BF6" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="BG6" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="BM6" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="BN6" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="BO6" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="BQ6" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="BR6" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="BS6" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="BU6" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="BV6" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="BW6" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="BY6" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="BZ6" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="CA6" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="CC6" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="CD6" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="CE6" s="10" t="s">
+        <v>339</v>
+      </c>
+      <c r="CO6" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="CP6" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="CQ6" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="CS6" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="CT6" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="CU6" s="10" t="s">
+        <v>397</v>
+      </c>
+      <c r="DA6" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="DB6" s="9" t="s">
+        <v>412</v>
+      </c>
+      <c r="DC6" s="10" t="s">
+        <v>413</v>
+      </c>
+      <c r="DI6" s="8" t="s">
+        <v>424</v>
+      </c>
+      <c r="DJ6" s="9" t="s">
+        <v>432</v>
+      </c>
+      <c r="DK6" s="10" t="s">
+        <v>433</v>
+      </c>
+      <c r="DQ6" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="DR6" s="9" t="s">
+        <v>448</v>
+      </c>
+      <c r="DS6" s="10" t="s">
+        <v>449</v>
+      </c>
+      <c r="DU6" t="s">
+        <v>450</v>
+      </c>
+      <c r="DV6" t="s">
+        <v>458</v>
+      </c>
+      <c r="DW6" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="7" spans="1:131" x14ac:dyDescent="0.35">
+      <c r="I7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="J7" s="9">
+        <v>3006</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="U7" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="V7" s="6">
+        <v>6006</v>
+      </c>
+      <c r="W7" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y7" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z7" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA7" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC7" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD7" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="AE7" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH7" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="AI7" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="AK7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL7" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="AM7" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="AS7" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="AT7" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="AU7" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="BE7" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="BF7" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="BG7" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="BM7" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="BN7" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="BO7" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="BQ7" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="BR7" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="BS7" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="CC7" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="CD7" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="CE7" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="CO7" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="CP7" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="CQ7" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="DA7" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="DB7" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="DC7" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="DU7" t="s">
+        <v>450</v>
+      </c>
+      <c r="DV7" t="s">
+        <v>460</v>
+      </c>
+      <c r="DW7" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="8" spans="1:131" x14ac:dyDescent="0.35">
+      <c r="Y8" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z8" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AA8" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC8" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD8" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="AE8" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH8" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="AI8" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="AK8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL8" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="AM8" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="AS8" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="AT8" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="AU8" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="BE8" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="BF8" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="BG8" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="BM8" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="BN8" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="BO8" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="BQ8" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="BR8" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="BS8" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="CC8" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="CD8" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="CE8" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="CO8" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="CP8" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="CQ8" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="DU8" t="s">
+        <v>450</v>
+      </c>
+      <c r="DV8" t="s">
+        <v>462</v>
+      </c>
+      <c r="DW8" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="9" spans="1:131" x14ac:dyDescent="0.35">
+      <c r="Y9" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z9" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA9" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC9" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD9" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="AE9" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH9" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="AI9" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="AK9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL9" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="AM9" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="AS9" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="AT9" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="AU9" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="BE9" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="BF9" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="BG9" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="BM9" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="BN9" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="BO9" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="BQ9" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="BR9" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="BS9" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="CC9" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="CD9" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="CE9" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="DU9" t="s">
+        <v>450</v>
+      </c>
+      <c r="DV9" t="s">
+        <v>464</v>
+      </c>
+      <c r="DW9" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="10" spans="1:131" x14ac:dyDescent="0.35">
+      <c r="AC10" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD10" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE10" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="AG10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH10" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="AI10" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="AK10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL10" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="AM10" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="AS10" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="AT10" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="AU10" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="BE10" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="BF10" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="BG10" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="BM10" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="BN10" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="BO10" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BQ10" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="BR10" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="BS10" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="CC10" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="CD10" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="CE10" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="DU10" t="s">
+        <v>450</v>
+      </c>
+      <c r="DV10" t="s">
+        <v>466</v>
+      </c>
+      <c r="DW10" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="11" spans="1:131" x14ac:dyDescent="0.35">
+      <c r="AC11" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD11" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="AE11" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH11" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="AI11" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="AK11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL11" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="AM11" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="AS11" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="AT11" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="AU11" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="BE11" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="BF11" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="BG11" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="BM11" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="BN11" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="BO11" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="BQ11" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="BR11" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="BS11" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="CC11" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="CD11" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="CE11" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="DU11" t="s">
+        <v>450</v>
+      </c>
+      <c r="DV11" t="s">
+        <v>468</v>
+      </c>
+      <c r="DW11" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="12" spans="1:131" x14ac:dyDescent="0.35">
+      <c r="AC12" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD12" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="AE12" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH12" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="AI12" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="AK12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL12" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="AM12" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="BE12" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="BF12" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="BG12" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="BM12" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="BN12" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="BO12" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="CC12" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="CD12" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="CE12" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="DU12" t="s">
+        <v>450</v>
+      </c>
+      <c r="DV12" t="s">
+        <v>470</v>
+      </c>
+      <c r="DW12" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="13" spans="1:131" x14ac:dyDescent="0.35">
+      <c r="AC13" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD13" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="AE13" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="AK13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL13" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="AM13" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="BE13" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="BF13" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="BG13" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="CC13" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="CD13" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="CE13" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="DU13" t="s">
+        <v>450</v>
+      </c>
+      <c r="DV13" t="s">
+        <v>472</v>
+      </c>
+      <c r="DW13" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="14" spans="1:131" x14ac:dyDescent="0.35">
+      <c r="AC14" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD14" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="AE14" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="AK14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL14" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="AM14" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="BE14" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="BF14" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="BG14" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="CC14" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="CD14" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="CE14" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="DU14" t="s">
+        <v>450</v>
+      </c>
+      <c r="DV14" t="s">
+        <v>474</v>
+      </c>
+      <c r="DW14" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="15" spans="1:131" x14ac:dyDescent="0.35">
+      <c r="AC15" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD15" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE15" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="AK15" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL15" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="AM15" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="BE15" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="BF15" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="BG15" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="CC15" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="CD15" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="CE15" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="DU15" t="s">
+        <v>450</v>
+      </c>
+      <c r="DV15" t="s">
+        <v>476</v>
+      </c>
+      <c r="DW15" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="16" spans="1:131" x14ac:dyDescent="0.35">
+      <c r="AC16" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD16" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="AE16" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AK16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL16" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="AM16" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="BE16" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="BF16" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="BG16" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="CC16" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="CD16" s="9" t="s">
+        <v>358</v>
+      </c>
+      <c r="CE16" s="10" t="s">
+        <v>359</v>
+      </c>
+      <c r="DU16" t="s">
+        <v>450</v>
+      </c>
+      <c r="DV16" t="s">
+        <v>478</v>
+      </c>
+      <c r="DW16" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="17" spans="29:127" x14ac:dyDescent="0.35">
+      <c r="AC17" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD17" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="AE17" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="CC17" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="CD17" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="CE17" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="DU17" t="s">
+        <v>450</v>
+      </c>
+      <c r="DV17" t="s">
+        <v>480</v>
+      </c>
+      <c r="DW17" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="18" spans="29:127" x14ac:dyDescent="0.35">
+      <c r="AC18" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD18" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="AE18" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="DU18" t="s">
+        <v>450</v>
+      </c>
+      <c r="DV18" t="s">
+        <v>482</v>
+      </c>
+      <c r="DW18" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="19" spans="29:127" x14ac:dyDescent="0.35">
+      <c r="AC19" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD19" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="AE19" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="DU19" t="s">
+        <v>450</v>
+      </c>
+      <c r="DV19" t="s">
+        <v>484</v>
+      </c>
+      <c r="DW19" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="20" spans="29:127" x14ac:dyDescent="0.35">
+      <c r="AC20" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD20" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="AE20" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="DU20" t="s">
+        <v>450</v>
+      </c>
+      <c r="DV20" t="s">
+        <v>486</v>
+      </c>
+      <c r="DW20" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="21" spans="29:127" x14ac:dyDescent="0.35">
+      <c r="AC21" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD21" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE21" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="DU21" t="s">
+        <v>450</v>
+      </c>
+      <c r="DV21" t="s">
+        <v>488</v>
+      </c>
+      <c r="DW21" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="22" spans="29:127" x14ac:dyDescent="0.35">
+      <c r="AC22" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD22" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="AE22" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="DU22" t="s">
+        <v>450</v>
+      </c>
+      <c r="DV22" t="s">
+        <v>490</v>
+      </c>
+      <c r="DW22" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="23" spans="29:127" x14ac:dyDescent="0.35">
+      <c r="AC23" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD23" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="AE23" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="DU23" t="s">
+        <v>450</v>
+      </c>
+      <c r="DV23" t="s">
+        <v>492</v>
+      </c>
+      <c r="DW23" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="24" spans="29:127" x14ac:dyDescent="0.35">
+      <c r="AC24" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD24" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="AE24" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="DU24" t="s">
+        <v>450</v>
+      </c>
+      <c r="DV24" t="s">
+        <v>494</v>
+      </c>
+      <c r="DW24" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="25" spans="29:127" x14ac:dyDescent="0.35">
+      <c r="AC25" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD25" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="AE25" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="DU25" t="s">
+        <v>450</v>
+      </c>
+      <c r="DV25" t="s">
+        <v>496</v>
+      </c>
+      <c r="DW25" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="26" spans="29:127" x14ac:dyDescent="0.35">
+      <c r="DU26" t="s">
+        <v>450</v>
+      </c>
+      <c r="DV26" t="s">
+        <v>498</v>
+      </c>
+      <c r="DW26" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="27" spans="29:127" x14ac:dyDescent="0.35">
+      <c r="DU27" t="s">
+        <v>450</v>
+      </c>
+      <c r="DV27" t="s">
+        <v>500</v>
+      </c>
+      <c r="DW27" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="28" spans="29:127" x14ac:dyDescent="0.35">
+      <c r="DU28" t="s">
+        <v>450</v>
+      </c>
+      <c r="DV28" t="s">
+        <v>502</v>
+      </c>
+      <c r="DW28" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="29" spans="29:127" x14ac:dyDescent="0.35">
+      <c r="DU29" t="s">
+        <v>450</v>
+      </c>
+      <c r="DV29" t="s">
+        <v>504</v>
+      </c>
+      <c r="DW29" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="30" spans="29:127" x14ac:dyDescent="0.35">
+      <c r="DU30" t="s">
+        <v>450</v>
+      </c>
+      <c r="DV30" t="s">
+        <v>506</v>
+      </c>
+      <c r="DW30" t="s">
+        <v>507</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Page: - User Role - User Setting - Warehouse: Add, Approve and Request
</commit_message>
<xml_diff>
--- a/InvSystem/obj/Release/Package/PackageTmp/template/TemplateUploadOri.xlsx
+++ b/InvSystem/obj/Release/Package/PackageTmp/template/TemplateUploadOri.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dede\WORK\Case\Inventory IT\Sample\Others\Sample\Empty\Final\InventorySystem\InvSystem\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\publisher\invpbs\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2626A0E7-5A51-47DD-910B-DB1027BCA5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC5ACAD-DB66-4DC7-9DB7-8A7EA77FC408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1D99F045-E079-4AC9-AE53-31F786CA0A7E}"/>
   </bookViews>
@@ -731,7 +731,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="513">
   <si>
     <t>AssetDesc</t>
   </si>
@@ -2263,10 +2263,13 @@
     <t>NA</t>
   </si>
   <si>
-    <t xml:space="preserve"> - </t>
-  </si>
-  <si>
-    <t>Dede Wahinime Antini</t>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Dede W. Antini</t>
+  </si>
+  <si>
+    <t>Syahri R. Putra</t>
   </si>
 </sst>
 </file>
@@ -2420,7 +2423,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{15E4EB1C-D8B0-4EA6-AFA0-9FCB4A23467D}" name="Table3" displayName="Table3" ref="DY1:EA3" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{15E4EB1C-D8B0-4EA6-AFA0-9FCB4A23467D}" name="Table3" displayName="Table3" ref="DY1:EA4" totalsRowShown="0">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{13509954-D920-4B99-AAB1-E3FB72BE0C8C}" name="Reference Type"/>
     <tableColumn id="2" xr3:uid="{98B4C5FF-CBDE-4B7D-A080-2C39F09A5B1B}" name="NIK"/>
@@ -3092,7 +3095,7 @@
   <dimension ref="A1:BC1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="J2" sqref="J2:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3477,7 +3480,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E2E0CB50-4087-47B7-BF44-BFBD9BCA0117}">
           <x14:formula1>
-            <xm:f>Sheet2!$DZ$2:$DZ$3</xm:f>
+            <xm:f>Sheet2!$DZ$2:$DZ$4</xm:f>
           </x14:formula1>
           <xm:sqref>J2:J1048576</xm:sqref>
         </x14:dataValidation>
@@ -3491,8 +3494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77814C16-67B4-433D-A132-47DC7CB73876}">
   <dimension ref="A1:EA30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="DO1" workbookViewId="0">
+      <selection activeCell="DZ9" sqref="DZ9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4719,6 +4722,15 @@
       <c r="DW4" t="s">
         <v>455</v>
       </c>
+      <c r="DY4" t="s">
+        <v>43</v>
+      </c>
+      <c r="DZ4">
+        <v>2020120171</v>
+      </c>
+      <c r="EA4" t="s">
+        <v>512</v>
+      </c>
     </row>
     <row r="5" spans="1:131" x14ac:dyDescent="0.35">
       <c r="A5" t="s">

</xml_diff>